<commit_message>
rename weighted Ja/Nein to weighted/unweighted. Some code refactors after more baseline experiments
</commit_message>
<xml_diff>
--- a/results/corpus_confront.xlsx
+++ b/results/corpus_confront.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrac\Documents\Uni\Embeddings\metaphor_experiment\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2487424-9C8F-41DA-A5AE-401EE4399B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06F54E9-70DF-4E13-BDB8-9CF545F01BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="250" yWindow="1140" windowWidth="18950" windowHeight="8920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="corpus_confront" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1478,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1489,10 +1502,10 @@
     <col min="4" max="4" width="16.54296875" customWidth="1"/>
     <col min="5" max="5" width="15.36328125" customWidth="1"/>
     <col min="6" max="6" width="15.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
+    <col min="8" max="8" width="16.08984375" customWidth="1"/>
+    <col min="9" max="9" width="26.26953125" customWidth="1"/>
+    <col min="10" max="10" width="23.1796875" customWidth="1"/>
     <col min="11" max="11" width="11.90625" customWidth="1"/>
     <col min="12" max="12" width="9.36328125" customWidth="1"/>
     <col min="13" max="13" width="11.90625" customWidth="1"/>

</xml_diff>